<commit_message>
EPBDS-8624 Fix backward compatibility
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8714_SmartRulesTRUEandFALSESupport.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8714_SmartRulesTRUEandFALSESupport.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A24116-4B77-4D20-B721-94252B6847A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="25875" windowHeight="11820"/>
+    <workbookView xWindow="3960" yWindow="2760" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="32">
   <si>
     <t>Return</t>
   </si>
@@ -27,9 +33,6 @@
     <t>SmartLookup Double myLookup(Integer a, Integer b, Integer c)</t>
   </si>
   <si>
-    <t>IsTrue</t>
-  </si>
-  <si>
     <t>=a&gt;b</t>
   </si>
   <si>
@@ -96,18 +99,12 @@
     <t>Is TRUE</t>
   </si>
   <si>
-    <t>Flase?</t>
-  </si>
-  <si>
     <t>flase</t>
   </si>
   <si>
     <t>rtue</t>
   </si>
   <si>
-    <t xml:space="preserve"> Truth</t>
-  </si>
-  <si>
     <t>SmartRules Double myTruth2(MyDatatype var)</t>
   </si>
   <si>
@@ -118,17 +115,19 @@
   </si>
   <si>
     <t>False?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> True</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,7 +151,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -163,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -190,7 +189,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -199,14 +198,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -244,9 +246,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,9 +281,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -314,9 +333,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -489,21 +525,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F8:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8:V8"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" width="20.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -513,10 +549,10 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="Q8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="6:21" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F9" t="b">
         <v>0</v>
       </c>
@@ -524,19 +560,19 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" t="s">
         <v>25</v>
       </c>
-      <c r="I9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" t="s">
-        <v>27</v>
-      </c>
       <c r="L9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M9" t="s">
         <v>0</v>
@@ -545,39 +581,39 @@
         <v>0</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="6:21" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -586,10 +622,10 @@
         <v>1</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T10" t="b">
         <v>0</v>
@@ -598,155 +634,155 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:21" x14ac:dyDescent="0.35">
       <c r="F11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M11">
         <v>2</v>
       </c>
       <c r="Q11" t="s">
+        <v>24</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="6:21" x14ac:dyDescent="0.35">
+      <c r="F12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>30</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T12" t="b">
+        <v>0</v>
+      </c>
+      <c r="U12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="6:21" x14ac:dyDescent="0.35">
+      <c r="F13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>31</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="6:21" x14ac:dyDescent="0.35">
+      <c r="Q14" t="s">
         <v>25</v>
       </c>
-      <c r="R11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="F12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>3</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>33</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="T12" t="b">
-        <v>0</v>
-      </c>
-      <c r="U12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="F13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>4</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="Q14" t="s">
-        <v>27</v>
-      </c>
       <c r="R14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="6:21" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="6:21" x14ac:dyDescent="0.35">
       <c r="Q15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T15" t="b">
         <v>0</v>
@@ -755,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:21" x14ac:dyDescent="0.35">
       <c r="Q16" t="s">
         <v>0</v>
       </c>
@@ -772,7 +808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F20" s="2" t="s">
         <v>2</v>
       </c>
@@ -781,12 +817,12 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -798,92 +834,92 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F22" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="F23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
         <v>7</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I23" t="s">
         <v>10</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" t="s">
+    <row r="24" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="F24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
         <v>8</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" t="s">
         <v>11</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
+    <row r="30" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="F30" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>16</v>
       </c>
-      <c r="G30" t="s">
+    </row>
+    <row r="31" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>18</v>
       </c>
-      <c r="G31" t="s">
+    </row>
+    <row r="32" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>20</v>
       </c>
-      <c r="G32" t="s">
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -896,24 +932,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>